<commit_message>
Fixed errors/Bugs. Completed switch from console Ai game to GUI AI game.  AI now works with the Unity GUI maze. Instructions are printed to the console for now(will be sound later) Moved files into better folders. changed Maze1.prefab to also hold its nodes and reset buttons.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Working on</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Getting Reset Button to reset player and all nodes and pathways</t>
+  </si>
+  <si>
+    <t>Converting  AI and Game to use GUI Nodes and paths for game</t>
   </si>
 </sst>
 </file>
@@ -466,16 +469,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -495,7 +498,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,6 +869,28 @@
       </c>
       <c r="C34" s="1">
         <v>41922</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>41923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Audio/scipt/dialogue for Ai. updated Capstone hours
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Working on</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>started at midnight</t>
+  </si>
+  <si>
+    <t>Writing Simple Ai Script</t>
+  </si>
+  <si>
+    <t>Recording Simple Ai Script</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +510,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -911,11 +917,28 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>0.5</v>
+      </c>
       <c r="C38" s="1">
         <v>41926</v>
       </c>
       <c r="D38" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>1.5</v>
+      </c>
+      <c r="C39" s="1">
+        <v>41926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got initial sound in and working. When audio is playing your can't go through doors, When you go through a door, the next instructions are played.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -135,13 +135,13 @@
     <t>Testing Unity Maze with AI, fixing bugs, fixing AI learning</t>
   </si>
   <si>
-    <t>started at midnight</t>
-  </si>
-  <si>
     <t>Writing Simple Ai Script</t>
   </si>
   <si>
     <t>Recording Simple Ai Script</t>
+  </si>
+  <si>
+    <t>Getting Simple Ai Script into the game.</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +493,7 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -510,7 +511,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>69</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -861,7 +862,7 @@
         <v>41921</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -872,7 +873,7 @@
         <v>41921</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -883,7 +884,7 @@
         <v>41922</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -894,7 +895,7 @@
         <v>41922</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -905,20 +906,20 @@
         <v>41923</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C37" s="1">
         <v>41923</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>0.5</v>
@@ -926,18 +927,26 @@
       <c r="C38" s="1">
         <v>41926</v>
       </c>
-      <c r="D38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>1.5</v>
       </c>
       <c r="C39" s="1">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
         <v>41926</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Neutrality is now in. Need to do more testing to see how well Ai does with such a small maze. For better results I think I will need a bigger maze. Trying to make a sound when jumping
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Working on</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Getting Simple Ai Script into the game.</t>
+  </si>
+  <si>
+    <t>Testing for Errors, Adding in Neutrality</t>
+  </si>
+  <si>
+    <t>Adding in jumping sound</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +517,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>72.5</v>
+        <v>74.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,6 +954,22 @@
       </c>
       <c r="C40" s="1">
         <v>41926</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding in New assets to use
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="11310"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="12435" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Working on</t>
   </si>
@@ -147,7 +147,31 @@
     <t>Testing for Errors, Adding in Neutrality</t>
   </si>
   <si>
-    <t>Adding in jumping sound</t>
+    <t>updating prefabs with nodes and pathchoices</t>
+  </si>
+  <si>
+    <t>Researching Random generation for mazes</t>
+  </si>
+  <si>
+    <t>Writing Story(prequel)</t>
+  </si>
+  <si>
+    <t>Fix movement sounds</t>
+  </si>
+  <si>
+    <t>Write Maze ending types(events that will happen and how they affect game)</t>
+  </si>
+  <si>
+    <t>finding models</t>
+  </si>
+  <si>
+    <t>Week 2 Hours</t>
+  </si>
+  <si>
+    <t>seting up models (textures, collision, scale, etc)</t>
+  </si>
+  <si>
+    <t>started at 12</t>
   </si>
 </sst>
 </file>
@@ -487,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,8 +540,8 @@
         <v>26</v>
       </c>
       <c r="F1">
-        <f>SUM(B2,B3:B300)</f>
-        <v>74.5</v>
+        <f>SUM(B2,B3:B301)</f>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,6 +572,13 @@
       <c r="C3" s="1">
         <v>41911</v>
       </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <f>SUM(B20:B43)</f>
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -931,7 +962,7 @@
         <v>0.5</v>
       </c>
       <c r="C38" s="1">
-        <v>41926</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,7 +973,7 @@
         <v>1.5</v>
       </c>
       <c r="C39" s="1">
-        <v>41926</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,7 +984,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="1">
-        <v>41926</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,12 +995,106 @@
         <v>2</v>
       </c>
       <c r="C41" s="1">
-        <v>41926</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>41925</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>41925</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>2.5</v>
+      </c>
+      <c r="C44" s="1">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="1">
+        <v>41926</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>41927</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1">
+        <v>41927</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>2.5</v>
+      </c>
+      <c r="C49" s="1">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="1">
+        <v>41929</v>
+      </c>
+      <c r="E50" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Hours. Moving on to making hallway prefabs
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Working on</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>seting up models (textures, collision, scale, etc)</t>
+  </si>
+  <si>
+    <t>Drawing new map</t>
+  </si>
+  <si>
+    <t>Drawing new map (Finished)</t>
+  </si>
+  <si>
+    <t>started at 1:30am</t>
+  </si>
+  <si>
+    <t>Making the new GUI Map</t>
+  </si>
+  <si>
+    <t>Designing new Node Travel</t>
+  </si>
+  <si>
+    <t>Making new Prefabs</t>
+  </si>
+  <si>
+    <t>1+</t>
+  </si>
+  <si>
+    <t>started at 3:30am</t>
   </si>
 </sst>
 </file>
@@ -508,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +562,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B301)</f>
-        <v>96.5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,7 +1096,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1107,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1092,6 +1116,55 @@
       </c>
       <c r="C50" s="1">
         <v>41929</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>41929</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>41930</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating hours --> Over 120 hours logged.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Working on</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Drawing new map (Finished)</t>
   </si>
   <si>
-    <t>Making the new GUI Map</t>
-  </si>
-  <si>
     <t>Designing new Node Travel</t>
   </si>
   <si>
@@ -195,10 +192,10 @@
     <t>Working on spawning Objects at end of the maze</t>
   </si>
   <si>
-    <t>started  at midnight</t>
-  </si>
-  <si>
     <t>Week 3 Hours</t>
+  </si>
+  <si>
+    <t>Fixing Bugs/Cleaning a bit of code</t>
   </si>
 </sst>
 </file>
@@ -540,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,8 +564,8 @@
         <v>26</v>
       </c>
       <c r="F1">
-        <f>SUM(B2,B3:B301)</f>
-        <v>119.5</v>
+        <f>SUM(B2,B3:B300)</f>
+        <v>123.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,7 +615,11 @@
         <v>41912</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B44:B60)</f>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,7 +1106,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>41929</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>41929</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1149,86 +1150,92 @@
         <v>41930</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>41931</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
         <v>41931</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="C55" s="1">
         <v>41931</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C56" s="1">
         <v>41931</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="1">
-        <v>41931</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41932</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="C58" s="1">
         <v>41932</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C59" s="1">
         <v>41932</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
       </c>
       <c r="C60" s="1">
-        <v>41933</v>
-      </c>
-      <c r="D60" t="s">
-        <v>59</v>
+        <v>41932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Options updated. Built new version. Loading/Saving NOT working fully. Check it out later!!!!
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Working on</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>138.5</v>
+        <v>150.5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,6 +1278,39 @@
       </c>
       <c r="C63" s="1">
         <v>41935</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" s="1">
+        <v>41936</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65" s="1">
+        <v>41937</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1">
+        <v>41938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Hours for Capstone. Now have over 215 hours of work.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>Working on</t>
   </si>
@@ -219,9 +219,6 @@
     <t>(lost one day)</t>
   </si>
   <si>
-    <t>(gained one day)</t>
-  </si>
-  <si>
     <t>Week 5 hours</t>
   </si>
   <si>
@@ -231,13 +228,37 @@
     <t>Disscusing plans about audio and improvements with team</t>
   </si>
   <si>
-    <t>started at 12am</t>
-  </si>
-  <si>
     <t xml:space="preserve">Getting Audio ready to be put in game/Putting in game </t>
   </si>
   <si>
-    <t>Putting in game/Optimizing Audio</t>
+    <t>Putting in game/Optimizing Audio/ Fixing Neutrality</t>
+  </si>
+  <si>
+    <t>Fixing Neutrality/Fixing Glitches/"Touching" up game</t>
+  </si>
+  <si>
+    <t>Making Graphs randomly Generated</t>
+  </si>
+  <si>
+    <t>Making Graphs randomly Generated &amp; fixing issues</t>
+  </si>
+  <si>
+    <t>fixing issues/bugs/cleaning up code</t>
+  </si>
+  <si>
+    <t>Adding Credits + above stuff</t>
+  </si>
+  <si>
+    <t>Working on Getting in End Game stuff</t>
+  </si>
+  <si>
+    <t>(gained one day + sick for one day)</t>
+  </si>
+  <si>
+    <t>Updating Options/Checking End Scene Works &amp; Fixing</t>
+  </si>
+  <si>
+    <t>2+</t>
   </si>
 </sst>
 </file>
@@ -577,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +628,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>172.5</v>
+        <v>218.25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -696,10 +717,14 @@
         <v>41913</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <f>SUM(B68:B78)</f>
+        <v>43.75</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1340,7 +1365,7 @@
         <v>41936</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -1351,7 +1376,7 @@
         <v>41937</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -1362,7 +1387,7 @@
         <v>41938</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -1373,9 +1398,9 @@
         <v>41939</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1384,9 +1409,9 @@
         <v>41939</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1395,7 +1420,7 @@
         <v>41939</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -1406,9 +1431,9 @@
         <v>41939</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71">
         <v>9</v>
@@ -1417,15 +1442,125 @@
         <v>41942</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
       </c>
       <c r="C72" s="1">
         <v>41943</v>
       </c>
-      <c r="D72" t="s">
-        <v>71</v>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>2.25</v>
+      </c>
+      <c r="C73" s="1">
+        <v>41945</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="C74" s="1">
+        <v>41945</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77" s="1">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78" s="1">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" s="1">
+        <v>41947</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>9</v>
+      </c>
+      <c r="C80" s="1">
+        <v>41948</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <v>5.5</v>
+      </c>
+      <c r="C81" s="1">
+        <v>41949</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" s="1">
+        <v>41950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest build of the game.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Working on</t>
   </si>
@@ -258,7 +258,10 @@
     <t>Updating Options/Checking End Scene Works &amp; Fixing</t>
   </si>
   <si>
-    <t>2+</t>
+    <t>Writing, Recording, putting in game new End Scene audio</t>
+  </si>
+  <si>
+    <t>Playtesting, Finding bugs, fixing fatal bugs that made game non-playable</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>218.25</v>
+        <v>229.25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1556,10 +1559,32 @@
       <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1">
+        <v>41950</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="1">
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" s="1">
+        <v>41950</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84">
+        <v>7</v>
+      </c>
+      <c r="C84" s="1">
         <v>41950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committed zipped file of game and time card.
</commit_message>
<xml_diff>
--- a/CapstoneHours.xlsx
+++ b/CapstoneHours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Working on</t>
   </si>
@@ -295,6 +295,33 @@
   </si>
   <si>
     <t>Recording Sound for Intro Cinema and getting it in</t>
+  </si>
+  <si>
+    <t>Trying to fix doors not using closed texture</t>
+  </si>
+  <si>
+    <t>Playtesting 2</t>
+  </si>
+  <si>
+    <t>Fixing and improving from Playtest2</t>
+  </si>
+  <si>
+    <t>Playtesting 2.1 - Playtesting with Jamies kid and getting feedback</t>
+  </si>
+  <si>
+    <t>Playtesting 2.2 - Playtesting with a couple of people</t>
+  </si>
+  <si>
+    <t>Smooth Camera turn</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Presentation+</t>
+  </si>
+  <si>
+    <t>11/29/2014 - 12/2/2014</t>
   </si>
 </sst>
 </file>
@@ -635,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +673,7 @@
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -665,7 +693,7 @@
       </c>
       <c r="F1">
         <f>SUM(B2,B3:B300)</f>
-        <v>268.75</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1778,6 +1806,116 @@
       </c>
       <c r="C97" s="1">
         <v>41960</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" s="1">
+        <v>41961</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="C99" s="1">
+        <v>41962</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100">
+        <v>7.25</v>
+      </c>
+      <c r="C100" s="1">
+        <v>41963</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>95</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101" s="1">
+        <v>41964</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>96</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" s="1">
+        <v>41964</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>95</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103" s="1">
+        <v>41966</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1">
+        <v>41967</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" s="1">
+        <v>41968</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>99</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" s="1">
+        <v>41969</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+      <c r="C107" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>